<commit_message>
voxxed done, some new talks confirmed
</commit_message>
<xml_diff>
--- a/TalksTable.xlsx
+++ b/TalksTable.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Privat\bernd-ruecker.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DFF511-903F-4C1D-82B8-EDA43D2719AB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10540" xr2:uid="{F5FCFEC6-B6BB-4038-B257-7F06F55ABB03}"/>
   </bookViews>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="212">
   <si>
     <t>Jfokus</t>
   </si>
@@ -550,9 +551,6 @@
     <t>Patience pays off. How long running services reduce complexity.</t>
   </si>
   <si>
-    <t>2018-03-12</t>
-  </si>
-  <si>
     <t>2018-05-09</t>
   </si>
   <si>
@@ -568,15 +566,9 @@
     <t>https://amsterdam2018.codemotionworld.com/talk-detail/?detail=7544</t>
   </si>
   <si>
-    <t>https://qconlondon.com/london2018/presentation/3-common-pitfalls-microservice-integration-and-how-avoid-them</t>
-  </si>
-  <si>
     <t>Qcon</t>
   </si>
   <si>
-    <t>2018-03-06</t>
-  </si>
-  <si>
     <t>http://java.withthebest.com/</t>
   </si>
   <si>
@@ -622,9 +614,6 @@
     <t>Break your event chains! Complex event flows in distributed systems.</t>
   </si>
   <si>
-    <t>https://voxxeddaysvienna2018.sched.com/event/Dl0C/patience-pays-off-how-long-running-services-reduce-complexity</t>
-  </si>
-  <si>
     <t>Nuremberg</t>
   </si>
   <si>
@@ -641,6 +630,39 @@
   </si>
   <si>
     <t>https://github.com/flowing/flowing-retail/</t>
+  </si>
+  <si>
+    <t>2018-03</t>
+  </si>
+  <si>
+    <t>www.jbcnconf.com/</t>
+  </si>
+  <si>
+    <t>3 common pitfalls in microservice integration and how to avoid them</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>JBCN Conf</t>
+  </si>
+  <si>
+    <t>2018-06-11</t>
+  </si>
+  <si>
+    <t>2018-06-21</t>
+  </si>
+  <si>
+    <t>Entwicklertag</t>
+  </si>
+  <si>
+    <t>Karlsruhe</t>
+  </si>
+  <si>
+    <t>http://entwicklertag.de/</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LJq6xAT0uwI</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01586060-4301-42D6-A296-5BF85ED0BBE5}">
-  <dimension ref="A2:N51"/>
+  <dimension ref="A2:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1076,28 +1098,22 @@
     </row>
     <row r="4" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>5</v>
+        <v>173</v>
+      </c>
+      <c r="H4" t="s">
+        <v>211</v>
       </c>
       <c r="L4" s="4" t="str">
         <f>IF(E4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
@@ -1105,34 +1121,37 @@
       </c>
       <c r="M4" s="3" t="str">
         <f>IF((LEN(G4)&gt;0),"&lt;a href='"&amp;G4&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H4)&gt;0),"&lt;a href='"&amp;H4&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I4)&gt;0),"&lt;a href='"&amp;I4&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J4)&gt;0),"&lt;a href='"&amp;J4&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://youtu.be/LJq6xAT0uwI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N6" si="0">IF(LEN(A4)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G4&amp;"'&gt;"&amp;F4&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B4&amp;" "&amp;L4&amp;" "&amp;C4&amp;" ("&amp;D4&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M4&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;2018-03-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Qcon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" ref="N4:N7" si="0">IF(LEN(A4)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G4&amp;"'&gt;"&amp;F4&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B4&amp;" "&amp;L4&amp;" "&amp;C4&amp;" ("&amp;D4&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M4&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;Patience pays off. How long running services reduce complexity.&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://youtu.be/LJq6xAT0uwI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>204</v>
+        <v>5</v>
       </c>
       <c r="L5" s="4" t="str">
         <f>IF(E5="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
@@ -1140,37 +1159,34 @@
       </c>
       <c r="M5" s="3" t="str">
         <f>IF((LEN(G5)&gt;0),"&lt;a href='"&amp;G5&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H5)&gt;0),"&lt;a href='"&amp;H5&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I5)&gt;0),"&lt;a href='"&amp;I5&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J5)&gt;0),"&lt;a href='"&amp;J5&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (New York City)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Qcon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="I6" t="s">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="L6" s="4" t="str">
         <f>IF(E6="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
@@ -1178,75 +1194,81 @@
       </c>
       <c r="M6" s="3" t="str">
         <f>IF((LEN(G6)&gt;0),"&lt;a href='"&amp;G6&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H6)&gt;0),"&lt;a href='"&amp;H6&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I6)&gt;0),"&lt;a href='"&amp;I6&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J6)&gt;0),"&lt;a href='"&amp;J6&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures'&gt;Lost in transaction - Strategies to deal with (in-)consistency in modern architectures&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (New York City)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>154</v>
+      <c r="B7" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
       </c>
       <c r="L7" s="4" t="str">
-        <f t="shared" ref="L7:L36" si="1">IF(E7="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f>IF(E7="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M7" s="3" t="str">
-        <f t="shared" ref="M7:M36" si="2">IF((LEN(G7)&gt;0),"&lt;a href='"&amp;G7&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H7)&gt;0),"&lt;a href='"&amp;H7&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I7)&gt;0),"&lt;a href='"&amp;I7&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J7)&gt;0),"&lt;a href='"&amp;J7&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <f>IF((LEN(G7)&gt;0),"&lt;a href='"&amp;G7&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H7)&gt;0),"&lt;a href='"&amp;H7&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I7)&gt;0),"&lt;a href='"&amp;I7&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J7)&gt;0),"&lt;a href='"&amp;J7&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" ref="N7:N51" si="3">IF(LEN(A7)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G7&amp;"'&gt;"&amp;F7&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B7&amp;" "&amp;L7&amp;" "&amp;C7&amp;" ("&amp;D7&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M7&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018'&gt;Microservices with Camunda&lt;/a&gt;&lt;p&gt;2018-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Camunda Days (Berlin, Hamburg, D&amp;uuml;sseldorf, Frankfurt, Munic,  Z&amp;uuml;rich, Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" si="0"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures'&gt;Lost in transaction - Strategies to deal with (in-)consistency in modern architectures&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <f t="shared" ref="L8:L37" si="1">IF(E8="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M8" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <f t="shared" ref="M8:M37" si="2">IF((LEN(G8)&gt;0),"&lt;a href='"&amp;G8&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H8)&gt;0),"&lt;a href='"&amp;H8&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I8)&gt;0),"&lt;a href='"&amp;I8&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J8)&gt;0),"&lt;a href='"&amp;J8&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale'&gt;Workflow Engines at scale&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" ref="N8:N52" si="3">IF(LEN(A8)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G8&amp;"'&gt;"&amp;F8&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B8&amp;" "&amp;L8&amp;" "&amp;C8&amp;" ("&amp;D8&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M8&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018'&gt;Microservices with Camunda&lt;/a&gt;&lt;p&gt;2018-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Camunda Days (Berlin, Hamburg, D&amp;uuml;sseldorf, Frankfurt, Munic,  Z&amp;uuml;rich, Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1263,10 +1285,10 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L9" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1274,11 +1296,11 @@
       </c>
       <c r="M9" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration'&gt;(Micro-)service collaboration&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale'&gt;Workflow Engines at scale&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1286,57 +1308,54 @@
         <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains'&gt;Break your event chains&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; MuCon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration'&gt;(Micro-)service collaboration&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="L11" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1344,11 +1363,11 @@
       </c>
       <c r="M11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow'&gt;Let your domain events flow&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; KanDDDinsky (Berlin), DDD Belgium (Gent), JCon (D&amp;uuml;sseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains'&gt;Break your event chains&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; MuCon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1356,22 +1375,22 @@
         <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L12" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1379,31 +1398,34 @@
       </c>
       <c r="M12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow'&gt;Let your domain events flow&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; KanDDDinsky (Berlin), DDD Belgium (Gent), JCon (D&amp;uuml;sseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
       </c>
       <c r="L13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1411,11 +1433,11 @@
       </c>
       <c r="M13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices'&gt;Orchestration of Microservices (Java edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JUG (Amsterdam), JUG  (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1423,31 +1445,31 @@
         <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices'&gt;Orchestration of Microservices (.NET edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices'&gt;Orchestration of Microservices (Java edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JUG (Amsterdam), JUG  (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1455,31 +1477,31 @@
         <v>157</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511'&gt;7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin), Java Forum Nord (Hannover)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices'&gt;Orchestration of Microservices (.NET edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1487,19 +1509,19 @@
         <v>157</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1507,11 +1529,11 @@
       </c>
       <c r="M16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows'&gt;Tackling complex event flows&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD Meetup (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511'&gt;7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin), Java Forum Nord (Hannover)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1519,66 +1541,63 @@
         <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
       </c>
       <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows'&gt;Tackling complex event flows&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD Meetup (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
         <v>58</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>59</v>
       </c>
-      <c r="L17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M17" s="3" t="str">
+      <c r="L18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
-      <c r="N17" t="str">
+      <c r="N18" t="str">
         <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBin (Trondheim, Bergen)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M18" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1586,13 +1605,13 @@
         <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>22</v>
@@ -1601,7 +1620,7 @@
         <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L19" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1609,11 +1628,11 @@
       </c>
       <c r="M19" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1633,80 +1652,80 @@
         <v>22</v>
       </c>
       <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
         <v>67</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="4" t="str">
+      <c r="L21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
-      <c r="M20" s="3" t="str">
+      <c r="M21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
-      <c r="N20" t="str">
+      <c r="N21" t="str">
         <f t="shared" si="3"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda'&gt;Business Rules with DMN&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" t="s">
-        <v>72</v>
-      </c>
-      <c r="L21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd'&gt;Long running processes in DDD&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD eXchange (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
     <row r="22" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
       <c r="B22" s="1" t="s">
         <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
       </c>
       <c r="L22" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1714,11 +1733,11 @@
       </c>
       <c r="M22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Goto Meetup (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd'&gt;Long running processes in DDD&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD eXchange (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1729,7 +1748,7 @@
         <v>160</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>74</v>
@@ -1738,10 +1757,10 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L23" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1749,11 +1768,11 @@
       </c>
       <c r="M23" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda'&gt;Open source workflow and rule management with Camunda&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBIn (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Goto Meetup (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1761,25 +1780,22 @@
         <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
-      </c>
-      <c r="J24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L24" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1787,11 +1803,11 @@
       </c>
       <c r="M24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than'&gt;Because your business is more complex than Netflix&lt;/a&gt;&lt;p&gt;2017-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda'&gt;Open source workflow and rule management with Camunda&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBIn (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1799,34 +1815,37 @@
         <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="J25" t="s">
+        <v>85</v>
       </c>
       <c r="L25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M25" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net'&gt;BPMN und Workflows in .NET - das geht!&lt;/a&gt;&lt;p&gt;2017-02 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than'&gt;Because your business is more complex than Netflix&lt;/a&gt;&lt;p&gt;2017-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1834,34 +1853,34 @@
         <v>60</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M26" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow'&gt;The 7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JFokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net'&gt;BPMN und Workflows in .NET - das geht!&lt;/a&gt;&lt;p&gt;2017-02 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1869,34 +1888,34 @@
         <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M27" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen'&gt;Prozesse digitalisieren - heute und morgen&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Digitalisierung und IT in Versicherungen  (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow'&gt;The 7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JFokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1907,34 +1926,31 @@
         <v>164</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="L28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm'&gt;Camunda BPM&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfall (Ede)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen'&gt;Prozesse digitalisieren - heute und morgen&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Digitalisierung und IT in Versicherungen  (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1945,28 +1961,34 @@
         <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" t="s">
+        <v>103</v>
       </c>
       <c r="L29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M29" s="3" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPMN &amp;amp; CMMN. Wann nehme ich welchen Standard?&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm'&gt;Camunda BPM&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfall (Ede)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1986,7 +2008,7 @@
         <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L30" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1998,7 +2020,7 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Gesch&amp;auml;ftsregeln mit DMN&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPMN &amp;amp; CMMN. Wann nehme ich welchen Standard?&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2006,22 +2028,19 @@
         <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
         <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
-      </c>
-      <c r="J31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L31" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2029,11 +2048,11 @@
       </c>
       <c r="M31" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v/>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Workflows mit BPMN 2.0 automatisieren&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Gesch&amp;auml;ftsregeln mit DMN&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2044,19 +2063,19 @@
         <v>165</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="J32" t="s">
+        <v>106</v>
       </c>
       <c r="L32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2064,11 +2083,11 @@
       </c>
       <c r="M32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action'&gt;Workflows (BPMN), Business Rules (DMN), Case Management (CMMN) – live &amp;amp; in Action&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Workflows mit BPMN 2.0 automatisieren&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2076,10 +2095,10 @@
         <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
         <v>54</v>
@@ -2088,10 +2107,10 @@
         <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>112</v>
-      </c>
-      <c r="J33" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="G33" t="s">
+        <v>109</v>
       </c>
       <c r="L33" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2099,11 +2118,11 @@
       </c>
       <c r="M33" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM und Microservices&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java EE Summit (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action'&gt;Workflows (BPMN), Business Rules (DMN), Case Management (CMMN) – live &amp;amp; in Action&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2114,19 +2133,19 @@
         <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
         <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="J34" t="s">
+        <v>113</v>
       </c>
       <c r="L34" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2134,11 +2153,11 @@
       </c>
       <c r="M34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+        <v>&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html'&gt;Workflows mit BPMN &amp;amp; Business Rules mit DMN - Open Source und in Action mit Camunda BPM (won best presentation award)&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM und Microservices&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java EE Summit (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2146,19 +2165,22 @@
         <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
         <v>22</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="G35" t="s">
+        <v>114</v>
       </c>
       <c r="L35" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2166,11 +2188,11 @@
       </c>
       <c r="M35" s="3" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM War Stories. Oder: Wie baue ich eine BPM-Architektur auf?&lt;/a&gt;&lt;p&gt;2016-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; SEACON (Hamburg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html'&gt;Workflows mit BPMN &amp;amp; Business Rules mit DMN - Open Source und in Action mit Camunda BPM (won best presentation award)&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2178,57 +2200,75 @@
         <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>118</v>
+      </c>
+      <c r="L36" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM War Stories. Oder: Wie baue ich eine BPM-Architektur auf?&lt;/a&gt;&lt;p&gt;2016-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; SEACON (Hamburg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>119</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>120</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>2</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>121</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
         <v>122</v>
       </c>
-      <c r="L36" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M36" s="3" t="str">
+      <c r="L37" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>&lt;a href='https://www.youtube.com/watch?v=x9ceAoZt8xw' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
-      <c r="N36" t="str">
+      <c r="N37" t="str">
         <f t="shared" si="3"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Open Source Workflows, Business Rules and Case Management live and in action&lt;/a&gt;&lt;p&gt;2015-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Devoxx (Antwerp)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=x9ceAoZt8xw' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L37" s="4" t="str">
-        <f t="shared" ref="L37:L51" si="4">IF(E37="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M37" s="3" t="str">
-        <f t="shared" ref="M37:M51" si="5">IF((LEN(G37)&gt;0),"&lt;a href='"&amp;G37&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H37)&gt;0),"&lt;a href='"&amp;H37&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I37)&gt;0),"&lt;a href='"&amp;I37&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J37)&gt;0),"&lt;a href='"&amp;J37&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v/>
-      </c>
-      <c r="N37" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L38" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L38:L52" si="4">IF(E38="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M38:M52" si="5">IF((LEN(G38)&gt;0),"&lt;a href='"&amp;G38&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H38)&gt;0),"&lt;a href='"&amp;H38&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I38)&gt;0),"&lt;a href='"&amp;I38&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J38)&gt;0),"&lt;a href='"&amp;J38&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
         <v/>
       </c>
       <c r="N38" t="str">
@@ -2418,15 +2458,28 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
+    <row r="52" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L52" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M52" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{B2CB20F6-AFDC-4220-B6CB-D765A8D94783}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{FDDD29D1-9830-4C9D-8735-D25A5B6DE6C7}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{900B2E3C-F4C2-487B-9C1E-A2369F22D279}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{01ADA2E4-A5C4-4E2E-BFCA-9E2B21411DFE}"/>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{B2CB20F6-AFDC-4220-B6CB-D765A8D94783}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{01ADA2E4-A5C4-4E2E-BFCA-9E2B21411DFE}"/>
+    <hyperlink ref="I4" r:id="rId3" display="https://github.com/flowing/flowing-retail/tree/master/payment-rest" xr:uid="{900B2E3C-F4C2-487B-9C1E-A2369F22D279}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2435,12 +2488,13 @@
   <dimension ref="A2:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.90625" style="1"/>
+    <col min="2" max="2" width="27.1796875" customWidth="1"/>
     <col min="8" max="8" width="10.90625" style="3"/>
   </cols>
   <sheetData>
@@ -2469,134 +2523,134 @@
     </row>
     <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" ref="H4:H47" si="0">IF(D4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I47" si="1">"&lt;tr&gt;&lt;td&gt;&lt;a href='"&amp;F4&amp;"'&gt;"&amp;E4&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B4&amp;" &lt;br&gt; "&amp;A4&amp;" "&amp;H4&amp;" "&amp;C4&amp;"&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://qconlondon.com/london2018/presentation/3-common-pitfalls-microservice-integration-and-how-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;Qcon &lt;br&gt; 2018-03-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; London&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/Domain-Driven-Design-Koln-Bonn/events/247273344/'&gt;Long-running services and Camunda &lt;/a&gt;&lt;p&gt;DDD Meetup &lt;br&gt; 2018-03-19 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Cologne&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F5" t="s">
-        <v>198</v>
+        <v>186</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://voxxeddaysvienna2018.sched.com/event/Dl0C/patience-pays-off-how-long-running-services-reduce-complexity'&gt;Patience pays off. How long running services reduce complexity.&lt;/a&gt;&lt;p&gt;Voxxed &lt;br&gt; 2018-03-12 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Vienna&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/jugthde/events/245462401/'&gt;Zeebe.io - Event-driven Microservice Orchestration&lt;/a&gt;&lt;p&gt;Java User Group &lt;br&gt; 2018-03-22 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Erfurt&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/Domain-Driven-Design-Koln-Bonn/events/247273344/'&gt;Long-running services and Camunda &lt;/a&gt;&lt;p&gt;DDD Meetup &lt;br&gt; 2018-03-19 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Cologne&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='http://java.withthebest.com/'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;Java With the Best &lt;br&gt; 2018-04-17 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Online&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/jugthde/events/245462401/'&gt;Zeebe.io - Event-driven Microservice Orchestration&lt;/a&gt;&lt;p&gt;Java User Group &lt;br&gt; 2018-03-22 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Erfurt&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://amsterdam2018.codemotionworld.com/talk-detail/?detail=7544'&gt;Workflow automation in the serverless age &lt;/a&gt;&lt;p&gt;Codemotion &lt;br&gt; 2018-05-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Amsterdam&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2604,27 +2658,27 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='http://java.withthebest.com/'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;Java With the Best &lt;br&gt; 2018-04-17 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Online&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://craft-conf.com/'&gt;Break your event chains! Complex event flows in distributed systems.&lt;/a&gt;&lt;p&gt;Craft-Conf &lt;br&gt; 2018-05-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Budapest&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2632,35 +2686,35 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://amsterdam2018.codemotionworld.com/talk-detail/?detail=7544'&gt;Workflow automation in the serverless age &lt;/a&gt;&lt;p&gt;Codemotion &lt;br&gt; 2018-05-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Amsterdam&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='www.jbcnconf.com/'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;JBCN Conf &lt;br&gt; 2018-06-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Barcelona&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://craft-conf.com/'&gt;Break your event chains! Complex event flows in distributed systems.&lt;/a&gt;&lt;p&gt;Craft-Conf &lt;br&gt; 2018-05-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Budapest&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='http://entwicklertag.de/'&gt;Lost in transaction? Über (In-)Kosistenz in verteilten Systemen &lt;/a&gt;&lt;p&gt;Entwicklertag &lt;br&gt; 2018-06-21 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Karlsruhe&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2671,7 +2725,7 @@
         <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -2699,7 +2753,7 @@
         <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -3074,15 +3128,16 @@
     <sortCondition ref="A4:A12"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{0E5527AD-E47A-49BF-AEF5-60BBFDC1A20E}"/>
-    <hyperlink ref="F9" r:id="rId2" xr:uid="{D5BB08EC-77FA-4C63-B367-DDD6BAFE2A89}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{50C94ACE-EFF7-458F-B729-7141A66F4830}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{94AD6036-1164-47A1-A88C-2BFA5E235597}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{82A9AD1D-FCBF-439E-B6AC-BF80A8905511}"/>
-    <hyperlink ref="F10" r:id="rId6" xr:uid="{C41C1E95-BB9A-459A-9124-471BE824E216}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{0E5527AD-E47A-49BF-AEF5-60BBFDC1A20E}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{D5BB08EC-77FA-4C63-B367-DDD6BAFE2A89}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{94AD6036-1164-47A1-A88C-2BFA5E235597}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{82A9AD1D-FCBF-439E-B6AC-BF80A8905511}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{C41C1E95-BB9A-459A-9124-471BE824E216}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{28AD5029-090C-46B0-ABE2-A7FB0B197E51}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{89DE3070-7D57-437F-BE86-164774E3AF22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed links, added recording from oreilly
</commit_message>
<xml_diff>
--- a/TalksTable.xlsx
+++ b/TalksTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Privat\bernd-ruecker.com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A0C6DC-F943-4647-B227-DEB01EAF509B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47033D3E-4D09-4E5E-A0AE-B02B5289928C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10540" xr2:uid="{F5FCFEC6-B6BB-4038-B257-7F06F55ABB03}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="217">
   <si>
     <t>Jfokus</t>
   </si>
@@ -44,9 +44,6 @@
     <t>https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures</t>
   </si>
   <si>
-    <t>https://github.com/flowing/flowing-retail/tree/master/payment-rest</t>
-  </si>
-  <si>
     <t>When</t>
   </si>
   <si>
@@ -671,10 +668,16 @@
     <t>https://www.youtube.com/watch?v=lZIe02um5eI</t>
   </si>
   <si>
-    <t>https://github.com/flowing/flowing-retail/tree/zeebe</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=AXgEowOgDSg</t>
+  </si>
+  <si>
+    <t>https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781492028116/video318624.html</t>
+  </si>
+  <si>
+    <t>https://github.com/flowing/flowing-retail/zeebe</t>
+  </si>
+  <si>
+    <t>https://github.com/flowing/rest/java/payment</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1064,7 @@
   <dimension ref="A2:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N4:N5"/>
+      <selection activeCell="N39" sqref="N4:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1072,108 +1075,108 @@
   <sheetData>
     <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
         <v>187</v>
       </c>
-      <c r="D4" t="s">
-        <v>188</v>
-      </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H4" t="s">
         <v>212</v>
       </c>
-      <c r="H4" t="s">
-        <v>213</v>
-      </c>
-      <c r="I4" t="s">
-        <v>214</v>
+      <c r="I4" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="L4" s="4" t="str">
-        <f>IF(E4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" ref="L4:L9" si="0">IF(E4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M4" s="3" t="str">
-        <f>IF((LEN(G4)&gt;0),"&lt;a href='"&amp;G4&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H4)&gt;0),"&lt;a href='"&amp;H4&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I4)&gt;0),"&lt;a href='"&amp;I4&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J4)&gt;0),"&lt;a href='"&amp;J4&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=lZIe02um5eI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/zeebe' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <f t="shared" ref="M4:M9" si="1">IF((LEN(G4)&gt;0),"&lt;a href='"&amp;G4&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H4)&gt;0),"&lt;a href='"&amp;H4&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I4)&gt;0),"&lt;a href='"&amp;I4&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J4)&gt;0),"&lt;a href='"&amp;J4&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=lZIe02um5eI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/zeebe' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N9" si="0">IF(LEN(A4)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G4&amp;"'&gt;"&amp;F4&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B4&amp;" "&amp;L4&amp;" "&amp;C4&amp;" ("&amp;D4&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M4&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration'&gt;Zeebe.io - Event-driven Microservice Orchestration&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java User Group (Erfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=lZIe02um5eI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/zeebe' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" ref="N4:N9" si="2">IF(LEN(A4)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G4&amp;"'&gt;"&amp;F4&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B4&amp;" "&amp;L4&amp;" "&amp;C4&amp;" ("&amp;D4&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M4&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration'&gt;Zeebe.io - Event-driven Microservice Orchestration&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java User Group (Erfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=lZIe02um5eI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/zeebe' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L5" s="4" t="str">
-        <f>IF(E5="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M5" s="3" t="str">
-        <f>IF((LEN(G5)&gt;0),"&lt;a href='"&amp;G5&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H5)&gt;0),"&lt;a href='"&amp;H5&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I5)&gt;0),"&lt;a href='"&amp;I5&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J5)&gt;0),"&lt;a href='"&amp;J5&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <f t="shared" si="1"/>
         <v>&lt;a href='https://www.youtube.com/watch?v=AXgEowOgDSg' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N5" t="str">
@@ -1183,112 +1186,115 @@
     </row>
     <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
         <v>81</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L6" s="4" t="str">
-        <f>IF(E6="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M6" s="3" t="str">
-        <f>IF((LEN(G6)&gt;0),"&lt;a href='"&amp;G6&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H6)&gt;0),"&lt;a href='"&amp;H6&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I6)&gt;0),"&lt;a href='"&amp;I6&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J6)&gt;0),"&lt;a href='"&amp;J6&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <f t="shared" si="1"/>
         <v>&lt;a href='https://youtu.be/LJq6xAT0uwI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;Patience pays off. How long running services reduce complexity.&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://youtu.be/LJq6xAT0uwI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="L7" s="4" t="str">
-        <f>IF(E7="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M7" s="3" t="str">
-        <f>IF((LEN(G7)&gt;0),"&lt;a href='"&amp;G7&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H7)&gt;0),"&lt;a href='"&amp;H7&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I7)&gt;0),"&lt;a href='"&amp;I7&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J7)&gt;0),"&lt;a href='"&amp;J7&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Qcon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Qcon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L8" s="4" t="str">
-        <f>IF(E8="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M8" s="3" t="str">
-        <f>IF((LEN(G8)&gt;0),"&lt;a href='"&amp;G8&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H8)&gt;0),"&lt;a href='"&amp;H8&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I8)&gt;0),"&lt;a href='"&amp;I8&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J8)&gt;0),"&lt;a href='"&amp;J8&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781492028116/video318624.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (New York City)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (New York City)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781492028116/video318624.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -1306,677 +1312,677 @@
         <v>4</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
+        <v>198</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="L9" s="4" t="str">
-        <f>IF(E9="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" si="0"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M9" s="3" t="str">
-        <f>IF((LEN(G9)&gt;0),"&lt;a href='"&amp;G9&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H9)&gt;0),"&lt;a href='"&amp;H9&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I9)&gt;0),"&lt;a href='"&amp;I9&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J9)&gt;0),"&lt;a href='"&amp;J9&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+        <f t="shared" si="1"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures'&gt;Lost in transaction - Strategies to deal with (in-)consistency in modern architectures&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/payment-rest' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures'&gt;Lost in transaction - Strategies to deal with (in-)consistency in modern architectures&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/user/javamattia' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
       <c r="L10" s="4" t="str">
-        <f t="shared" ref="L10:L39" si="1">IF(E10="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" ref="L10:L39" si="3">IF(E10="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M10" s="3" t="str">
-        <f t="shared" ref="M10:M39" si="2">IF((LEN(G10)&gt;0),"&lt;a href='"&amp;G10&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H10)&gt;0),"&lt;a href='"&amp;H10&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I10)&gt;0),"&lt;a href='"&amp;I10&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J10)&gt;0),"&lt;a href='"&amp;J10&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <f t="shared" ref="M10:M39" si="4">IF((LEN(G10)&gt;0),"&lt;a href='"&amp;G10&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H10)&gt;0),"&lt;a href='"&amp;H10&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I10)&gt;0),"&lt;a href='"&amp;I10&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J10)&gt;0),"&lt;a href='"&amp;J10&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" ref="N10:N54" si="3">IF(LEN(A10)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G10&amp;"'&gt;"&amp;F10&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B10&amp;" "&amp;L10&amp;" "&amp;C10&amp;" ("&amp;D10&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M10&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="N10:N54" si="5">IF(LEN(A10)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G10&amp;"'&gt;"&amp;F10&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B10&amp;" "&amp;L10&amp;" "&amp;C10&amp;" ("&amp;D10&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M10&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018'&gt;Microservices with Camunda&lt;/a&gt;&lt;p&gt;2018-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Camunda Days (Berlin, Hamburg, D&amp;uuml;sseldorf, Frankfurt, Munic,  Z&amp;uuml;rich, Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" t="s">
-        <v>23</v>
-      </c>
       <c r="L11" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M11" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale'&gt;Workflow Engines at scale&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
       <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
       <c r="L12" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M12" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration'&gt;(Micro-)service collaboration&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
         <v>29</v>
       </c>
-      <c r="G13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" t="s">
-        <v>30</v>
-      </c>
       <c r="L13" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M13" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains'&gt;Break your event chains&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; MuCon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
         <v>34</v>
       </c>
-      <c r="H14" t="s">
-        <v>35</v>
-      </c>
       <c r="L14" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M14" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow'&gt;Let your domain events flow&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; KanDDDinsky (Berlin), DDD Belgium (Gent), JCon (D&amp;uuml;sseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
         <v>38</v>
       </c>
-      <c r="G15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" t="s">
-        <v>39</v>
-      </c>
       <c r="L15" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M15" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
         <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M16" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices'&gt;Orchestration of Microservices (Java edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JUG (Amsterdam), JUG  (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L17" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M17" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices'&gt;Orchestration of Microservices (.NET edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
         <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
       </c>
       <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="G18" t="s">
-        <v>52</v>
-      </c>
       <c r="L18" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M18" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511'&gt;7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin), Java Forum Nord (Hannover)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
         <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L19" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M19" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows'&gt;Tackling complex event flows&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD Meetup (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
       </c>
       <c r="F20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" t="s">
         <v>58</v>
       </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
       <c r="L20" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M20" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBin (Trondheim, Bergen)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>61</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
         <v>62</v>
       </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>63</v>
       </c>
-      <c r="G21" t="s">
-        <v>64</v>
-      </c>
       <c r="L21" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M21" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" t="s">
         <v>65</v>
       </c>
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>66</v>
-      </c>
       <c r="L22" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M22" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" t="s">
         <v>67</v>
       </c>
-      <c r="G23" t="s">
-        <v>68</v>
-      </c>
       <c r="L23" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M23" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda'&gt;Business Rules with DMN&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
       </c>
       <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>71</v>
       </c>
-      <c r="H24" t="s">
-        <v>72</v>
-      </c>
       <c r="L24" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M24" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd'&gt;Long running processes in DDD&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD eXchange (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
         <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>74</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L25" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M25" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Goto Meetup (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
         <v>2</v>
       </c>
       <c r="F26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" t="s">
         <v>79</v>
       </c>
-      <c r="G26" t="s">
-        <v>80</v>
-      </c>
       <c r="L26" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda'&gt;Open source workflow and rule management with Camunda&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBIn (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
         <v>81</v>
-      </c>
-      <c r="D27" t="s">
-        <v>82</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" t="s">
         <v>83</v>
       </c>
-      <c r="G27" t="s">
+      <c r="J27" t="s">
         <v>84</v>
       </c>
-      <c r="J27" t="s">
-        <v>85</v>
-      </c>
       <c r="L27" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M27" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than'&gt;Because your business is more complex than Netflix&lt;/a&gt;&lt;p&gt;2017-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="s">
         <v>86</v>
       </c>
-      <c r="G28" t="s">
-        <v>87</v>
-      </c>
       <c r="L28" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M28" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net'&gt;BPMN und Workflows in .NET - das geht!&lt;/a&gt;&lt;p&gt;2017-02 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
@@ -1985,577 +1991,412 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" t="s">
         <v>89</v>
       </c>
-      <c r="G29" t="s">
-        <v>90</v>
-      </c>
       <c r="L29" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M29" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow'&gt;The 7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JFokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
         <v>91</v>
       </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>92</v>
       </c>
-      <c r="G30" t="s">
-        <v>93</v>
-      </c>
       <c r="L30" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M30" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen'&gt;Prozesse digitalisieren - heute und morgen&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Digitalisierung und IT in Versicherungen  (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" t="s">
-        <v>100</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
       </c>
       <c r="F31" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" t="s">
         <v>101</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>102</v>
       </c>
-      <c r="H31" t="s">
-        <v>103</v>
-      </c>
       <c r="L31" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M31" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm'&gt;Camunda BPM&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfall (Ede)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s">
         <v>20</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>21</v>
       </c>
-      <c r="E32" t="s">
-        <v>22</v>
-      </c>
       <c r="F32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L32" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPMN &amp;amp; CMMN. Wann nehme ich welchen Standard?&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
         <v>20</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>21</v>
       </c>
-      <c r="E33" t="s">
-        <v>22</v>
-      </c>
       <c r="F33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L33" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M33" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Gesch&amp;auml;ftsregeln mit DMN&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" t="s">
         <v>105</v>
       </c>
-      <c r="J34" t="s">
-        <v>106</v>
-      </c>
       <c r="L34" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M34" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Workflows mit BPMN 2.0 automatisieren&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" t="s">
         <v>108</v>
       </c>
-      <c r="D35" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" t="s">
-        <v>109</v>
-      </c>
       <c r="L35" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M35" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action'&gt;Workflows (BPMN), Business Rules (DMN), Case Management (CMMN) – live &amp;amp; in Action&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
         <v>111</v>
       </c>
-      <c r="D36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="J36" t="s">
         <v>112</v>
       </c>
-      <c r="J36" t="s">
-        <v>113</v>
-      </c>
       <c r="L36" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M36" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM und Microservices&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java EE Summit (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>61</v>
       </c>
-      <c r="D37" t="s">
-        <v>62</v>
-      </c>
       <c r="E37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L37" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M37" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html'&gt;Workflows mit BPMN &amp;amp; Business Rules mit DMN - Open Source und in Action mit Camunda BPM (won best presentation award)&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" t="s">
         <v>115</v>
       </c>
-      <c r="D38" t="s">
-        <v>116</v>
-      </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L38" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM War Stories. Oder: Wie baue ich eine BPM-Architektur auf?&lt;/a&gt;&lt;p&gt;2016-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; SEACON (Hamburg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" t="s">
         <v>119</v>
-      </c>
-      <c r="D39" t="s">
-        <v>120</v>
       </c>
       <c r="E39" t="s">
         <v>2</v>
       </c>
       <c r="F39" t="s">
+        <v>120</v>
+      </c>
+      <c r="I39" t="s">
         <v>121</v>
       </c>
-      <c r="I39" t="s">
-        <v>122</v>
-      </c>
       <c r="L39" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="M39" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>&lt;a href='https://www.youtube.com/watch?v=x9ceAoZt8xw' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Open Source Workflows, Business Rules and Case Management live and in action&lt;/a&gt;&lt;p&gt;2015-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Devoxx (Antwerp)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=x9ceAoZt8xw' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L40" s="4" t="str">
-        <f t="shared" ref="L40:L54" si="4">IF(E40="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M40" s="3" t="str">
-        <f t="shared" ref="M40:M54" si="5">IF((LEN(G40)&gt;0),"&lt;a href='"&amp;G40&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H40)&gt;0),"&lt;a href='"&amp;H40&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I40)&gt;0),"&lt;a href='"&amp;I40&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J40)&gt;0),"&lt;a href='"&amp;J40&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
-        <v/>
-      </c>
-      <c r="N40" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L41" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M41" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N41" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L42" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M42" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N42" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L43" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M43" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N43" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L44" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M44" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N44" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L44" s="4"/>
     </row>
     <row r="45" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L45" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M45" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N45" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L46" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M46" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N46" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L47" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M47" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N47" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L47" s="4"/>
     </row>
     <row r="48" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L48" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M48" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N48" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="49" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L49" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M49" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N49" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="50" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L50" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M50" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N50" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="51" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L51" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M51" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N51" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="52" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L52" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M52" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N52" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="53" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L53" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M53" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N53" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="54" spans="12:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L54" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
-      </c>
-      <c r="M54" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N54" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;&lt;/a&gt;&lt;p&gt; &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;  ()&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L54" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2563,9 +2404,12 @@
     <hyperlink ref="I8" r:id="rId2" xr:uid="{01ADA2E4-A5C4-4E2E-BFCA-9E2B21411DFE}"/>
     <hyperlink ref="I6" r:id="rId3" display="https://github.com/flowing/flowing-retail/tree/master/payment-rest" xr:uid="{900B2E3C-F4C2-487B-9C1E-A2369F22D279}"/>
     <hyperlink ref="I5" r:id="rId4" xr:uid="{D288DED8-2D4A-4F87-B3DF-8F1BD0D7FF9F}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{649CD0D6-9E06-4F22-BCA5-E80C1821530E}"/>
+    <hyperlink ref="I4" r:id="rId6" xr:uid="{B48AFA3B-6513-4CDF-B2AB-ADEF13504FCB}"/>
+    <hyperlink ref="I9" r:id="rId7" display="https://github.com/flowing/flowing-retail/tree/master/payment-rest" xr:uid="{97E748A2-734B-477E-8503-72C10E428AE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2586,45 +2430,45 @@
   <sheetData>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" ref="H4:H47" si="0">IF(D4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
@@ -2637,22 +2481,22 @@
     </row>
     <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
         <v>187</v>
       </c>
-      <c r="C5" t="s">
-        <v>188</v>
-      </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2665,22 +2509,22 @@
     </row>
     <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2693,22 +2537,22 @@
     </row>
     <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
         <v>174</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>175</v>
-      </c>
-      <c r="C7" t="s">
-        <v>176</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2721,22 +2565,22 @@
     </row>
     <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" t="s">
         <v>191</v>
-      </c>
-      <c r="C8" t="s">
-        <v>192</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2749,22 +2593,22 @@
     </row>
     <row r="9" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2777,22 +2621,22 @@
     </row>
     <row r="10" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" t="s">
         <v>207</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>208</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2805,22 +2649,22 @@
     </row>
     <row r="11" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2833,22 +2677,22 @@
     </row>
     <row r="12" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3243,42 +3087,42 @@
   <sheetData>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H4" s="4" t="str">
         <f>IF(D4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
@@ -3291,19 +3135,19 @@
     </row>
     <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
         <v>127</v>
-      </c>
-      <c r="C5" t="s">
-        <v>128</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" ref="H5:H11" si="0">IF(D5="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
@@ -3316,19 +3160,19 @@
     </row>
     <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
         <v>131</v>
-      </c>
-      <c r="F6" t="s">
-        <v>132</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3341,22 +3185,22 @@
     </row>
     <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3369,22 +3213,22 @@
     </row>
     <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" t="s">
         <v>139</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
         <v>140</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>141</v>
-      </c>
-      <c r="F8" t="s">
-        <v>142</v>
       </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3397,22 +3241,22 @@
     </row>
     <row r="9" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
         <v>143</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
         <v>144</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>145</v>
-      </c>
-      <c r="F9" t="s">
-        <v>146</v>
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3425,22 +3269,22 @@
     </row>
     <row r="10" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>147</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>148</v>
-      </c>
-      <c r="F10" t="s">
-        <v>149</v>
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3453,19 +3297,19 @@
     </row>
     <row r="11" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
         <v>152</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>153</v>
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
added lost-in-transaction page and missing images
</commit_message>
<xml_diff>
--- a/TalksTable.xlsx
+++ b/TalksTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Privat\berndruecker.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594977FA-5DA6-44D1-BCA8-B2E584357E1C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3221DE-75F9-4040-995B-5071D755D78D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25613" windowHeight="10553" xr2:uid="{F5FCFEC6-B6BB-4038-B257-7F06F55ABB03}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10550" activeTab="1" xr2:uid="{F5FCFEC6-B6BB-4038-B257-7F06F55ABB03}"/>
   </bookViews>
   <sheets>
     <sheet name="Recent talks" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="325">
   <si>
     <t>Jfokus</t>
   </si>
@@ -996,6 +996,18 @@
   </si>
   <si>
     <t>https://dddeurope.com/2019/</t>
+  </si>
+  <si>
+    <t>2018-01-08</t>
+  </si>
+  <si>
+    <t>https://www.meetup.com/JUG-Bonn/events/255097835/</t>
+  </si>
+  <si>
+    <t>Bonn</t>
+  </si>
+  <si>
+    <t>JUG Bonn</t>
   </si>
 </sst>
 </file>
@@ -3339,18 +3351,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01586060-4301-42D6-A296-5BF85ED0BBE5}">
   <dimension ref="A2:N84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.796875" style="1"/>
-    <col min="3" max="3" width="17.19921875" customWidth="1"/>
-    <col min="12" max="13" width="10.796875" style="3"/>
+    <col min="2" max="2" width="10.81640625" style="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="12" max="13" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -3388,7 +3400,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G3" s="5"/>
       <c r="L3" s="4"/>
       <c r="M3" s="3" t="str">
@@ -3396,7 +3408,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>315</v>
       </c>
@@ -3434,7 +3446,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls of microservice integration&lt;/a&gt;&lt;p&gt;2018-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; MuCon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/12766-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>315</v>
       </c>
@@ -3469,7 +3481,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls of microservice integration&lt;/a&gt;&lt;p&gt;2018-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>306</v>
       </c>
@@ -3504,7 +3516,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://conferences.oreilly.com/software-architecture/sa-eu/public/schedule/detail/69841'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://conferences.oreilly.com/software-architecture/sa-eu/public/schedule/detail/69841' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>306</v>
       </c>
@@ -3539,7 +3551,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/gophercon-uk-2018-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; GoLab (Florence)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/gophercon-uk-2018-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>306</v>
       </c>
@@ -3577,7 +3589,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kafka-summit-2018-monitoring-and-orchestration-of-your-microservices-landscape-with-zeebe'&gt;Monitoring and Orchestration of Your Microservices Landscape with Kafka and Zeebe&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Apache Kafka Meetup Berlin (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kafka-summit-2018-monitoring-and-orchestration-of-your-microservices-landscape-with-zeebe' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/iXkM-X6Kihk' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>306</v>
       </c>
@@ -3615,7 +3627,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kafka-summit-2018-monitoring-and-orchestration-of-your-microservices-landscape-with-zeebe'&gt;The Big Picture: Monitoring and Orchestration of Your Microservices Landscape with Kafka and Zeebe &lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Kafka Summit (San Francisco)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kafka-summit-2018-monitoring-and-orchestration-of-your-microservices-landscape-with-zeebe' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.confluent.io/kafka-summit-sf18/the_big_picture' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>306</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JCon (Dusseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>306</v>
       </c>
@@ -3679,7 +3691,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Strategies to deal with (in-)consistency in distributed systems.&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JCon (Dusseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>306</v>
       </c>
@@ -3714,7 +3726,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JAX (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://jaxenter.com/microservices-interview-ruecker-jax-london-151031.html' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>306</v>
       </c>
@@ -3752,7 +3764,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/Microservices-Meetup-Munich/events/253329558/'&gt;Double Feature: Events and long running services&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Microservices Meetup (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/Microservices-Meetup-Munich/events/253329558/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=7xC3dUIvF-0' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>289</v>
       </c>
@@ -3790,7 +3802,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://skillsmatter.com/conferences/10160-cloudnative-london-2018#program'&gt;Coordinate cloud-native components using distributed state machines&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Cloud Native (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://skillsmatter.com/conferences/10160-cloudnative-london-2018#program' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/12110-coordinate-cloud-native-components-using-distributed-state-machines' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>289</v>
       </c>
@@ -3825,7 +3837,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='http://devconf.pl/#schedule2_day2_auditorium1_time3'&gt;Complex Event Flows in Distributed Systems&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DevConf (Krakow)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='http://devconf.pl/#schedule2_day2_auditorium1_time3' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=EegrVoPTRbQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>289</v>
       </c>
@@ -3863,7 +3875,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Strategies to deal with (in-)consistency in distributed systems&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaZone Noway (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://2018.javazone.no/program/45df84d4-e819-4fc9-9e3b-931972891441' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>289</v>
       </c>
@@ -3898,7 +3910,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java Forum Nord (Hannover)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>289</v>
       </c>
@@ -3934,7 +3946,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Strategies to deal with (in-)consistency in distributed systems&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Full Stack Fest (Barcelona)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=JtaoNlL5mdI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>289</v>
       </c>
@@ -3969,7 +3981,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://basta.net/microservices-apis/kommunikation-zwischen-microservices/'&gt;Kommunikation zwischen Microservices&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://basta.net/microservices-apis/kommunikation-zwischen-microservices/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>289</v>
       </c>
@@ -4001,7 +4013,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://basta.net/web-development/workflows-mit-bpmn-automatisieren-lessons-learned/'&gt;Workflows mit BPMN automatisieren. Lessons Learned.&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://basta.net/web-development/workflows-mit-bpmn-automatisieren-lessons-learned/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>289</v>
       </c>
@@ -4033,7 +4045,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/JUG-Mainz/events/249130598/'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JUG (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/JUG-Mainz/events/249130598/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Über (In-)Kosistenz in verteilten Systemen&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Herbstcampus (Nurremberg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>288</v>
       </c>
@@ -4109,7 +4121,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/gophercon-uk-2018-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2018-08 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; GopherCon  (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/gophercon-uk-2018-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=NBo7d5AG-3s' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/rest/go' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; The New York City Java Meetup Group (New York)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>221</v>
       </c>
@@ -4179,7 +4191,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/complex-event-flows-in-distributed-systems'&gt;Complex Event Flows in Distributed Systems&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; QCon (New York)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.infoq.com/presentations/event-flow-distributed-systems' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; QCon (New York)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -4246,7 +4258,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Lost in transaction? Über (In-)Kosistenz in verteilten Systemen &lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Entwicklertag (Karlsruhe)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -4281,7 +4293,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/workflow-automation-with-bpmn-lessons-learned'&gt;Workflows mit BPMN automatisieren. Lessons Learned.&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Developer Week (Nuremberg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/workflow-automation-with-bpmn-lessons-learned' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -4316,7 +4328,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Lost in transaction? Strategies to deal with (in-)consistency in modern architectures.&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Devoxx Poland (Krakow)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?list=PLRsbF2sD7JVrSMm9aK4juBQz9AyU_rakc&amp;v=8KgTB75VePo' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -4351,7 +4363,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration'&gt;3 common pitfalls in microservice integration and how to avoid them&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JBCN Conf (Barcelona)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/3-common-pitfalls-in-microservice-integration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>226</v>
       </c>
@@ -4380,7 +4392,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;Workflow automation in the serverless age &lt;/a&gt;&lt;p&gt;2018-05 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Codemotion (Amsterdam)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>226</v>
       </c>
@@ -4415,7 +4427,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://speakerdeck.com/martinschimak/craftconf-budapest-2018-break-your-event-chains-complex-event-flows-in-distributed-systems'&gt;Break your event chains! Complex event flows in distributed systems.&lt;/a&gt;&lt;p&gt;2018-05 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Craft-Conf (Budapest)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://speakerdeck.com/martinschimak/craftconf-budapest-2018-break-your-event-chains-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.ustream.tv/recorded/114862863' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -4450,7 +4462,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;2018-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Java With the Best (Online)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -4491,7 +4503,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration'&gt;Zeebe.io - Event-driven Microservice Orchestration&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java User Group (Erfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/java-user-group-erfurt-2018-zeebeio-eventdriven-microservice-orchestration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=lZIe02um5eI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/zeebe' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -4529,7 +4541,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Long-running services and Camunda &lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; DDD Meetup (Cologne)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=AXgEowOgDSg' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -4564,7 +4576,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Patience pays off. How long running services reduce complexity.&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://youtu.be/LJq6xAT0uwI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>187</v>
       </c>
@@ -4602,7 +4614,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them'&gt;3 Common Pitfalls in Microservice Integration and How to Avoid them&lt;/a&gt;&lt;p&gt;2018-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Qcon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/qcon-london-2018-3-common-pitfalls-in-microservice-integration-and-how-to-avoid-them' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://youtu.be/O2-NHptllKQ' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>123</v>
       </c>
@@ -4640,7 +4652,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (New York City)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-nyc-2018-complex-event-flows-in-distributed-systems/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781492028116/video318624.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>123</v>
       </c>
@@ -4678,7 +4690,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures'&gt;Lost in transaction - Strategies to deal with (in-)consistency in modern architectures&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=Ikj59uEKhjg' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>242</v>
       </c>
@@ -4713,7 +4725,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018'&gt;Microservices with Camunda&lt;/a&gt;&lt;p&gt;2018-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Camunda Days (Berlin, Hamburg, D&amp;uuml;sseldorf, Frankfurt, Munic,  Z&amp;uuml;rich, Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/microservices-with-camunda-talk-from-camunda-days-012018' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>242</v>
       </c>
@@ -4748,7 +4760,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale'&gt;Workflow Engines at scale&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-workflow-and-state-machines-at-scale' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -4783,7 +4795,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration'&gt;(Micro-)service collaboration&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/wjax-2017-microservice-collaboration' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -4821,7 +4833,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains'&gt;Break your event chains&lt;/a&gt;&lt;p&gt;2017-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; MuCon (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/mucon-london-2017-break-your-event-chains' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/10718-break-your-event-chains' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>154</v>
       </c>
@@ -4856,7 +4868,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow'&gt;Let your domain events flow&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; KanDDDinsky (Berlin), DDD Belgium (Gent), JCon (D&amp;uuml;sseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/kandddinsky-let-your-domain-events-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=LKoaMbqZp9Y' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -4894,7 +4906,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems'&gt;Complex event flows in distributed systems&lt;/a&gt;&lt;p&gt;2017-10 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; O'Reilly Software Architecture (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/oreilly-sa-complex-event-flows-in-distributed-systems' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.safaribooksonline.com/library/view/oreilly-software-architecture/9781491985274/video315427.html' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -4929,7 +4941,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices'&gt;Orchestration of Microservices (Java edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JUG (Amsterdam), JUG  (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jug-frankfurt-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -4967,7 +4979,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices'&gt;Orchestration of Microservices (.NET edition)&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/basta-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=4g2drf_EjWk' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -5002,7 +5014,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511'&gt;7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin), Java Forum Nord (Hannover)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/7-sins-of-workflow-80009511' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -5037,7 +5049,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows'&gt;Tackling complex event flows&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD Meetup (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2017-0905-ddd-ber-tackling-complex-event-flows' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -5072,7 +5084,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBin (Trondheim, Bergen)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-trondheim-and-bergen-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -5107,7 +5119,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfs-2017-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -5142,7 +5154,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices'&gt;Orchestration of Microservices&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-orchestration-of-microservices' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -5177,7 +5189,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda'&gt;Business Rules with DMN&lt;/a&gt;&lt;p&gt;2017-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JAX (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jax-2017-talk-business-rules-with-dmn-and-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>158</v>
       </c>
@@ -5212,7 +5224,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd'&gt;Long running processes in DDD&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; DDD eXchange (London)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/long-running-processes-in-ddd' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://skillsmatter.com/skillscasts/9853-long-running-processes-in-ddd' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -5247,7 +5259,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow'&gt;Let your microservices flow&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Goto Meetup (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/goto-meetup-stockholm-let-your-microservices-flow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -5282,7 +5294,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda'&gt;Open source workflow and rule management with Camunda&lt;/a&gt;&lt;p&gt;2017-04 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaBIn (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/javabin-oslo-open-source-workflow-and-rule-management-with-camunda' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -5320,7 +5332,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than'&gt;Because your business is more complex than Netflix&lt;/a&gt;&lt;p&gt;2017-03 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Voxxed (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/master-the-flow-of-microservices-because-your-business-is-more-complex-than' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.voxxed.com/blog/2017/03/orchestration-stacks-netflix/' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -5355,7 +5367,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net'&gt;BPMN und Workflows in .NET - das geht!&lt;/a&gt;&lt;p&gt;2017-02 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Frankfurt)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/bpmn-und-workflows-in-net' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -5390,7 +5402,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow'&gt;The 7 sins of workflow&lt;/a&gt;&lt;p&gt;2017-01 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JFokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/the-7-sins-of-workflow' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -5425,7 +5437,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen'&gt;Prozesse digitalisieren - heute und morgen&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Digitalisierung und IT in Versicherungen  (Vienna)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/prozesse-digitalisieren-heute-und-morgen' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -5463,7 +5475,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm'&gt;Camunda BPM&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfall (Ede)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-jfall-camunda-bpm' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=_WKlc_X6zNE' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -5495,7 +5507,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPMN &amp;amp; CMMN. Wann nehme ich welchen Standard?&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -5527,7 +5539,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Gesch&amp;auml;ftsregeln mit DMN&lt;/a&gt;&lt;p&gt;2016-11 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; WJAX (Munic)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>59</v>
       </c>
@@ -5562,7 +5574,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Workflows mit BPMN 2.0 automatisieren&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Basta (Mainz)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=LTQtwHdBrr8' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -5597,7 +5609,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action'&gt;Workflows (BPMN), Business Rules (DMN), Case Management (CMMN) – live &amp;amp; in Action&lt;/a&gt;&lt;p&gt;2016-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; BedCon (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://de.slideshare.net/BerndRuecker/2016-bedcon-talk-workflows-bpmn-business-rules-dmn-case-management-cmmn-live-in-action' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -5632,7 +5644,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM und Microservices&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java EE Summit (Berlin)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=Up4QcVHxrwA' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>59</v>
       </c>
@@ -5667,7 +5679,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html'&gt;Workflows mit BPMN &amp;amp; Business Rules mit DMN - Open Source und in Action mit Camunda BPM (won best presentation award)&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JFS (Stuttgart)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='http://www.java-forum-stuttgart.de/de/BestPresentations+2016.html' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -5699,7 +5711,7 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;BPM War Stories. Oder: Wie baue ich eine BPM-Architektur auf?&lt;/a&gt;&lt;p&gt;2016-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; SEACON (Hamburg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -5734,49 +5746,49 @@
         <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Open Source Workflows, Business Rules and Case Management live and in action&lt;/a&gt;&lt;p&gt;2015-11 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Devoxx (Antwerp)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?v=x9ceAoZt8xw' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L70" s="4"/>
     </row>
-    <row r="71" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L71" s="4"/>
     </row>
-    <row r="72" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L73" s="4"/>
     </row>
-    <row r="74" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L77" s="4"/>
     </row>
-    <row r="78" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L80" s="4"/>
     </row>
-    <row r="81" spans="12:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L81" s="4"/>
     </row>
-    <row r="82" spans="12:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L82" s="4"/>
     </row>
-    <row r="83" spans="12:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L83" s="4"/>
     </row>
-    <row r="84" spans="12:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="12:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L84" s="4"/>
     </row>
   </sheetData>
@@ -5854,20 +5866,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DED00E-46E1-48BC-B1F1-251D95106922}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.796875" style="1"/>
-    <col min="2" max="2" width="27.19921875" customWidth="1"/>
-    <col min="8" max="8" width="10.796875" style="3"/>
+    <col min="1" max="1" width="10.81640625" style="1"/>
+    <col min="2" max="2" width="27.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -5890,7 +5902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>311</v>
       </c>
@@ -5918,7 +5930,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://dvbe18.confinabox.com/talk/BIP-8983/3_common_pitfalls_in_microservice_integration_and_how_to_avoid_them'&gt;3 common pitfalls of microservice integration&lt;/a&gt;&lt;p&gt;Devoxx &lt;br&gt; 2018-11-15 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Antwerp&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>263</v>
       </c>
@@ -5944,7 +5956,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;3 common pitfalls of microservice integration&lt;/a&gt;&lt;p&gt;Codemotion &lt;br&gt; 2018-11-20 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Berlin&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>264</v>
       </c>
@@ -5970,7 +5982,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;3 common pitfalls of microservice integration&lt;/a&gt;&lt;p&gt;DOAG &lt;br&gt; 2018-11-21 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Nurremberg&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>254</v>
       </c>
@@ -5998,7 +6010,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.versicherungsforen.net/portal/de/messekongresse/it/index.xhtml'&gt;Ein Kessel Buntes – BPM(N) Anwendungsszenarien bei der Allianz&lt;/a&gt;&lt;p&gt;IT for insurances &lt;br&gt; 2018-11-27 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Leipzig&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>247</v>
       </c>
@@ -6026,7 +6038,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.dotnet-developer-conference.de/programm/#/tag-3'&gt;3 common pitfalls in microservice integration&lt;/a&gt;&lt;p&gt;.NET Developer Conference &lt;br&gt; 2018-11-28 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Cologne&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>203</v>
       </c>
@@ -6054,7 +6066,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='http://www.jug-muenster.de/'&gt;Zeebe.io - New Open Source Project for event-driven Microservice Orchestration&lt;/a&gt;&lt;p&gt;JUG Münster &lt;br&gt; 2018-12-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Muenster&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>275</v>
       </c>
@@ -6082,7 +6094,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/Domain-Driven-Design-Ruhrgebiet/events/253263745/'&gt;Live Coding around Process Managers, Sagas and Orchestration&lt;/a&gt;&lt;p&gt;DDD Meetup &lt;br&gt; 2018-12-06 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Essen&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>238</v>
       </c>
@@ -6102,136 +6114,165 @@
         <v>235</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f t="shared" ref="H10:H12" si="2">IF(D10="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <f t="shared" ref="H10:H13" si="2">IF(D10="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
         <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" ref="I10:I12" si="3">"&lt;tr&gt;&lt;td&gt;&lt;a href='"&amp;F10&amp;"'&gt;"&amp;E10&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B10&amp;" &lt;br&gt; "&amp;A10&amp;" "&amp;H10&amp;" "&amp;C10&amp;"&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="I10:I13" si="3">"&lt;tr&gt;&lt;td&gt;&lt;a href='"&amp;F10&amp;"'&gt;"&amp;E10&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B10&amp;" &lt;br&gt; "&amp;A10&amp;" "&amp;H10&amp;" "&amp;C10&amp;"&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.ittage.informatik-aktuell.de/'&gt;3 typische Stolperfallen bei der Microservice-Integration&lt;/a&gt;&lt;p&gt;IT Tage &lt;br&gt; 2018-12-10 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Frankfurt&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>323</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>318</v>
+        <v>248</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://dddeurope.com/2019/'&gt;Lost in transaction? Strategies to manage consistency across boundaries &lt;/a&gt;&lt;p&gt;DDD Europe &lt;br&gt; 2019-01-31 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Amsterdam&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.meetup.com/JUG-Bonn/events/255097835/'&gt;3 common pitfalls in microservice integration&lt;/a&gt;&lt;p&gt;JUG Bonn &lt;br&gt; 2018-01-08 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Bonn&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="C12" t="s">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="3"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://dddeurope.com/2019/'&gt;Lost in transaction? Strategies to manage consistency across boundaries &lt;/a&gt;&lt;p&gt;DDD Europe &lt;br&gt; 2019-01-31 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Amsterdam&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://programm.javaland.eu/2019/#/scheduledEvent/569570'&gt;Lost in Transaction? Data Consistency in Distributed Systems&lt;/a&gt;&lt;p&gt;Java Land &lt;br&gt; 2019-03-19 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Brühl&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="8:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H29" s="4"/>
     </row>
+    <row r="30" spans="8:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="4"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:G31">
-    <sortCondition ref="A2:A31"/>
+  <sortState ref="A2:G32">
+    <sortCondition ref="A2:A32"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{7B88BBA1-9E52-44D7-AC6F-10682A6F2BE8}"/>
     <hyperlink ref="F7" r:id="rId2" location="/tag-3" xr:uid="{810E31D0-4440-4E0A-88EA-FFF9EB1F1D1D}"/>
     <hyperlink ref="F10" r:id="rId3" xr:uid="{2B26B471-EE23-4CAD-845A-1FCB2A15F06E}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{387628AD-8DFE-4C52-A652-25D066974691}"/>
-    <hyperlink ref="F12" r:id="rId5" location="/scheduledEvent/569570" xr:uid="{7DCE906A-D09C-40AF-BD3B-42768CEBE40A}"/>
+    <hyperlink ref="F13" r:id="rId5" location="/scheduledEvent/569570" xr:uid="{7DCE906A-D09C-40AF-BD3B-42768CEBE40A}"/>
     <hyperlink ref="F3" r:id="rId6" xr:uid="{61C4C08F-A2AE-4738-9E3C-C197686947B7}"/>
-    <hyperlink ref="F11" r:id="rId7" xr:uid="{671A6070-534C-404E-99B2-0365CD56558F}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{671A6070-534C-404E-99B2-0365CD56558F}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{2CB493EA-DCD2-4F06-B1B6-609A3406AA08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -6243,13 +6284,13 @@
       <selection activeCell="I4" sqref="I4:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.55" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.796875" style="1"/>
-    <col min="8" max="8" width="10.796875" style="3"/>
+    <col min="2" max="2" width="10.81640625" style="1"/>
+    <col min="8" max="8" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -6272,7 +6313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>210</v>
       </c>
@@ -6293,7 +6334,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://thenewstack.io/5-workflow-automation-use-cases-you-might-not-have-considered/'&gt;5 Workflow Automation Use Cases You Might Not Have Considered&lt;/a&gt;&lt;p&gt;2018-04  TheNewStack&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>123</v>
       </c>
@@ -6318,7 +6359,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.infoworld.com/article/3254777/application-development/3-common-pitfalls-of-microservices-integrationand-how-to-avoid-them.html'&gt;3 common pitfalls of microservices integration—and how to avoid them&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; InfoWorld&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>125</v>
       </c>
@@ -6343,7 +6384,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.infoq.com/articles/events-workflow-automation'&gt;Events, Flows and Long-Running Services: A Modern Approach to Workflow Automation&lt;/a&gt;&lt;p&gt;2017-12 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; InfoQ&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>131</v>
       </c>
@@ -6368,7 +6409,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.infoq.com/articles/microservice-event-choreographies'&gt;Know the Flow! Microservices and Event Choreographies&lt;/a&gt;&lt;p&gt;2017-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; InfoQ&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -6396,7 +6437,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://entwickler.de/online/windowsdeveloper/workflows-bpmn-automatisieren-301118.html'&gt;Workflows mit BPMN effektiv automatisieren&lt;/a&gt;&lt;p&gt;2016-10 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Windows Developer&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6424,7 +6465,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://network.camunda.org/whitepaper/45'&gt;BPM macht Spaß&lt;/a&gt;&lt;p&gt;2016-07 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java Aktuell&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -6452,7 +6493,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.sigs-datacom.de/uploads/tx_dmjournals/ruecker_OS_05_16_TRBT.pdf'&gt;Decision Model and Notation: Digitalisierung von Entscheidungen mit DMN&lt;/a&gt;&lt;p&gt;2016-05 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Objekt Spektrum&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -6480,7 +6521,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://jaxenter.de/der-brueckenschlag-warum-dmn-den-business-rules-engines-markt-aufmischt-37252'&gt;Der Brückenschlag: Warum DMN den Business-Rules-Engines-Markt aufmischt&lt;/a&gt;&lt;p&gt;2016-04 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Business Technology&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -6505,7 +6546,7 @@
         <v>&lt;tr&gt;&lt;td&gt;&lt;a href=''&gt;Quo Vadis BPM&lt;/a&gt;&lt;p&gt;2016-01 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Java Magazin&lt;/p&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H13" s="4" t="str">
         <f t="shared" ref="H13:H49" si="2">IF(D13="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6515,7 +6556,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H14" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6525,7 +6566,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H15" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6535,7 +6576,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H16" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6545,7 +6586,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="17" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H17" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6555,7 +6596,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="18" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H18" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6565,7 +6606,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="19" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H19" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6575,7 +6616,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H20" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6585,7 +6626,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H21" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6595,7 +6636,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="22" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6605,7 +6646,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="23" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H23" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6615,7 +6656,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="24" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H24" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6625,7 +6666,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6635,7 +6676,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="26" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H26" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6645,7 +6686,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="27" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H27" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6655,7 +6696,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="28" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H28" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6665,7 +6706,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="29" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H29" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6675,7 +6716,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="30" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H30" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6685,7 +6726,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="31" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H31" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6695,7 +6736,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="32" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H32" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6705,7 +6746,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="33" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H33" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6715,7 +6756,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H34" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6725,7 +6766,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="35" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H35" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6735,7 +6776,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="36" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H36" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6745,7 +6786,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="37" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H37" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6755,7 +6796,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="38" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H38" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6765,7 +6806,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="39" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H39" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6775,7 +6816,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="40" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H40" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6785,7 +6826,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="41" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H41" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6795,7 +6836,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="42" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H42" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6805,7 +6846,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="43" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H43" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6815,7 +6856,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="44" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H44" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6825,7 +6866,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="45" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H45" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6835,7 +6876,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="46" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H46" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6845,7 +6886,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="47" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H47" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6855,7 +6896,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="48" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H48" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6865,7 +6906,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="49" spans="8:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="8:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="H49" s="4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
@@ -6889,17 +6930,17 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.46484375" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>267</v>
       </c>
@@ -6907,7 +6948,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>268</v>
       </c>
@@ -6915,7 +6956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>269</v>
       </c>
@@ -6927,7 +6968,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>279</v>
       </c>
@@ -6935,7 +6976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>270</v>
       </c>
@@ -6943,7 +6984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -6951,7 +6992,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>272</v>
       </c>
@@ -6959,7 +7000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>278</v>
       </c>
@@ -6967,7 +7008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -6975,7 +7016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>277</v>
       </c>
@@ -6983,7 +7024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>271</v>
       </c>
@@ -6991,7 +7032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B25">
         <f>SUM(B19:B24)</f>
         <v>41</v>

</xml_diff>

<commit_message>
updated homepage and added talk overview pages and refactored out bio
</commit_message>
<xml_diff>
--- a/TalksTable.xlsx
+++ b/TalksTable.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Privat\berndruecker.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3221DE-75F9-4040-995B-5071D755D78D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB67828-4300-4890-903E-07D2CBBD485B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10550" activeTab="1" xr2:uid="{F5FCFEC6-B6BB-4038-B257-7F06F55ABB03}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="10550" activeTab="4" xr2:uid="{F5FCFEC6-B6BB-4038-B257-7F06F55ABB03}"/>
   </bookViews>
   <sheets>
     <sheet name="Recent talks" sheetId="1" r:id="rId1"/>
     <sheet name="Upcoming talks" sheetId="2" r:id="rId2"/>
     <sheet name="Articles" sheetId="3" r:id="rId3"/>
     <sheet name="Stats" sheetId="4" r:id="rId4"/>
+    <sheet name="Recent talks Lost In TX" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="325">
   <si>
     <t>Jfokus</t>
   </si>
@@ -1072,7 +1074,27 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5793,10 +5815,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N4:N70">
-    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
+    <cfRule type="uniqueValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+    <cfRule type="uniqueValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G38" r:id="rId1" xr:uid="{B2CB20F6-AFDC-4220-B6CB-D765A8D94783}"/>
@@ -5868,8 +5890,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6258,7 +6280,7 @@
       <c r="H30" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">
     <sortCondition ref="A2:A32"/>
   </sortState>
   <hyperlinks>
@@ -7039,10 +7061,438 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="L20:L62">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L20:L62">
     <sortCondition ref="L20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED18AEB-249F-4A03-8E91-7150780898CF}">
+  <dimension ref="A2:N25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4:N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" style="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="12" max="13" width="10.90625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="3" t="str">
+        <f t="shared" ref="M3:M10" si="0">IF((LEN(G3)&gt;0),"&lt;a href='"&amp;G3&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H3)&gt;0),"&lt;a href='"&amp;H3&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I3)&gt;0),"&lt;a href='"&amp;I3&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J3)&gt;0),"&lt;a href='"&amp;J3&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="L4" s="4" t="str">
+        <f t="shared" ref="L4" si="1">IF(E4="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4" si="2">IF(LEN(A4)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G4&amp;"'&gt;"&amp;F4&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B4&amp;" "&amp;L4&amp;" "&amp;C4&amp;" ("&amp;D4&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M4&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Strategies to deal with (in-)consistency in distributed systems.&lt;/a&gt;&lt;p&gt;2018-10 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; JCon (Dusseldorf)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="L5" s="4" t="str">
+        <f t="shared" ref="L5:L10" si="3">IF(E5="de","&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;","&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;")</f>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M5" s="3" t="str">
+        <f t="shared" ref="M5:M10" si="4">IF((LEN(G5)&gt;0),"&lt;a href='"&amp;G5&amp;"' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(H5)&gt;0),"&lt;a href='"&amp;H5&amp;"' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;", "") &amp;IF((LEN(I5)&gt;0),"&lt;a href='"&amp;I5&amp;"' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;","")&amp;IF((LEN(J5)&gt;0),"&lt;a href='"&amp;J5&amp;"' title='Interview'&gt;&lt;img src='assets/img/interview.png' height='20px'&gt;&lt;/a&gt;","")</f>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://2018.javazone.no/program/45df84d4-e819-4fc9-9e3b-931972891441' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" ref="N5:N10" si="5">IF(LEN(A5)&gt;0,"&lt;tr class='additional-row'&gt;","&lt;tr&gt;")&amp;"&lt;td&gt;&lt;a href='"&amp;G5&amp;"'&gt;"&amp;F5&amp;"&lt;/a&gt;&lt;p&gt;"&amp;B5&amp;" "&amp;L5&amp;" "&amp;C5&amp;" ("&amp;D5&amp;")&lt;/p&gt;&lt;/td&gt;&lt;td&gt;" &amp;M5&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Strategies to deal with (in-)consistency in distributed systems&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; JavaZone Noway (Oslo)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://2018.javazone.no/program/45df84d4-e819-4fc9-9e3b-931972891441' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="L6" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M6" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=JtaoNlL5mdI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Strategies to deal with (in-)consistency in distributed systems&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Full Stack Fest (Barcelona)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=JtaoNlL5mdI' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="L7" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M7" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/'&gt;Lost in transaction? Über (In-)Kosistenz in verteilten Systemen&lt;/a&gt;&lt;p&gt;2018-09 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Herbstcampus (Nurremberg)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/2018-lost-in-transaction/' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/berndruecker/flowing-retail' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>167</v>
+      </c>
+      <c r="L8" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M8" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Lost in transaction? Über (In-)Kosistenz in verteilten Systemen &lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In German language'&gt;&lt;img src='assets/img/de.png' height='20px'&gt;&lt;/span&gt; Entwicklertag (Karlsruhe)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>224</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="L9" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M9" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;a href='https://www.youtube.com/watch?list=PLRsbF2sD7JVrSMm9aK4juBQz9AyU_rakc&amp;v=8KgTB75VePo' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr class='additional-row'&gt;&lt;td&gt;&lt;a href=''&gt;Lost in transaction? Strategies to deal with (in-)consistency in modern architectures.&lt;/a&gt;&lt;p&gt;2018-06 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Devoxx Poland (Krakow)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.youtube.com/watch?list=PLRsbF2sD7JVrSMm9aK4juBQz9AyU_rakc&amp;v=8KgTB75VePo' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="L10" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt;</v>
+      </c>
+      <c r="M10" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=Ikj59uEKhjg' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="5"/>
+        <v>&lt;tr&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures'&gt;Lost in transaction - Strategies to deal with (in-)consistency in modern architectures&lt;/a&gt;&lt;p&gt;2018-02 &lt;span title='In English language'&gt;&lt;img src='assets/img/en.png' height='20px'&gt;&lt;/span&gt; Jfokus (Stockholm)&lt;/p&gt;&lt;/td&gt;&lt;td&gt;&lt;a href='https://www.slideshare.net/BerndRuecker/jfokus-2018-lost-in-transaction-strategies-to-deal-with-inconsistency-in-modern-architectures' title='Slides'&gt;&lt;img src='assets/img/slides.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://www.youtube.com/watch?v=Ikj59uEKhjg' title='Recording'&gt;&lt;img src='assets/img/recording.png' height='20px'&gt;&lt;/a&gt;&lt;a href='https://github.com/flowing/flowing-retail/tree/master/rest/java/payment' title='Source code'&gt;&lt;img src='assets/img/code.png' height='20px'&gt;&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22"/>
+      <c r="B22" s="1"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22" s="4"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23"/>
+      <c r="B23" s="1"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23" s="4"/>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24"/>
+      <c r="B24" s="1"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24" s="4"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="1:14" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25"/>
+      <c r="B25" s="1"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25" s="4"/>
+      <c r="N25"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N11">
+    <cfRule type="uniqueValues" dxfId="0" priority="10"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="I10" r:id="rId1" display="https://github.com/flowing/flowing-retail/tree/master/payment-rest" xr:uid="{EDA107AA-E164-4054-8EAD-88829DD70192}"/>
+    <hyperlink ref="H10" r:id="rId2" xr:uid="{FFBB8390-048A-493A-BB75-BCADFC5F5E76}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{A2D426E2-335C-47FF-836B-B3BDB7FB575D}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{B8FF3A48-BF39-4E7E-B245-EF9CE0303C27}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{CD4AAD50-E0C6-4C9F-B3C6-77EBC7499511}"/>
+    <hyperlink ref="H5" r:id="rId6" xr:uid="{CF4AE815-D2DC-430C-8ECA-65816F051572}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{D2C287DF-F2B7-49FD-8C43-4B2C12CDCE4B}"/>
+    <hyperlink ref="H6" r:id="rId8" xr:uid="{2307D982-0AAD-4ACC-89DE-94FA529F926C}"/>
+    <hyperlink ref="I5" r:id="rId9" xr:uid="{8D61C17C-3C99-45C5-B75A-609F4A13705A}"/>
+    <hyperlink ref="I7" r:id="rId10" xr:uid="{5B2A9383-E173-4F54-9D76-AFB372A62652}"/>
+    <hyperlink ref="G4" r:id="rId11" xr:uid="{CC7739A1-0E3E-41C7-9A9C-4151602D453B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
+</worksheet>
 </file>
</xml_diff>